<commit_message>
asset production year, insurance page table
</commit_message>
<xml_diff>
--- a/public/template/TemplateAsset.xlsx
+++ b/public/template/TemplateAsset.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Asset Number</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Asset Name ID</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -74,16 +71,7 @@
     <t>Acquisition Value</t>
   </si>
   <si>
-    <t>Current Cost</t>
-  </si>
-  <si>
-    <t>Useful Life Month</t>
-  </si>
-  <si>
-    <t>Accumulate Depre</t>
-  </si>
-  <si>
-    <t>Net Book Value</t>
+    <t>Production Year</t>
   </si>
 </sst>
 </file>
@@ -448,23 +436,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.77734375" customWidth="1"/>
     <col min="11" max="11" width="12.88671875" customWidth="1"/>
     <col min="12" max="12" width="15.109375" customWidth="1"/>
@@ -472,13 +460,9 @@
     <col min="14" max="14" width="15.88671875" customWidth="1"/>
     <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,46 +488,33 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix import, logo export
</commit_message>
<xml_diff>
--- a/public/template/TemplateAsset.xlsx
+++ b/public/template/TemplateAsset.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Asset Number</t>
   </si>
   <si>
-    <t>Asset Name ID</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -53,12 +50,6 @@
     <t>PO No.</t>
   </si>
   <si>
-    <t>Location ID</t>
-  </si>
-  <si>
-    <t>Department ID</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -80,9 +71,6 @@
     <t>FA1323520100012 (Required)</t>
   </si>
   <si>
-    <t>64 (Required)</t>
-  </si>
-  <si>
     <t>Kawasaki KLX 150G (Required)</t>
   </si>
   <si>
@@ -104,9 +92,6 @@
     <t>EBB202212008 (Opsional)</t>
   </si>
   <si>
-    <t>2 (Required)</t>
-  </si>
-  <si>
     <t>1 (Required)</t>
   </si>
   <si>
@@ -117,6 +102,24 @@
   </si>
   <si>
     <t>12/1/2022 (Required)</t>
+  </si>
+  <si>
+    <t>Asset Name</t>
+  </si>
+  <si>
+    <t>Motor cycle (Required)</t>
+  </si>
+  <si>
+    <t>Mantimin (Required)</t>
+  </si>
+  <si>
+    <t>HRGA (Required)</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Department</t>
   </si>
 </sst>
 </file>
@@ -497,13 +500,13 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
@@ -512,7 +515,7 @@
     <col min="8" max="8" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.109375" customWidth="1"/>
     <col min="13" max="13" width="10.88671875" customWidth="1"/>
     <col min="14" max="14" width="20.44140625" customWidth="1"/>
@@ -525,99 +528,99 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="N2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>